<commit_message>
Natively support new shorthand relationship symbols.
</commit_message>
<xml_diff>
--- a/vdd/tests/data/demo_model.xlsx
+++ b/vdd/tests/data/demo_model.xlsx
@@ -304,21 +304,25 @@
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J6" activeCellId="0" sqref="J6"/>
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.4336734693878"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.93877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="3.6530612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="5.04081632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="4.47959183673469"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="5.04081632653061"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="3.6530612244898"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="4.47959183673469"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="4.06632653061225"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="5.04081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="3.6530612244898"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="4.47959183673469"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="3.6530612244898"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="5.04081632653061"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="3.6530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>